<commit_message>
[fixes] - fixed "quiet mode" ([`nexial.quiet`]) so that console logs will be drastically reduced.
(improvements)
- [`project.properties`]: supports environment-specific project.properties via runtime environment variable `nexial.env`.
  - when environment-specific project.properties is specified, the default `project.properties` will be loaded first
- minor log reformatting to improve readability.

Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_project_properties.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_project_properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\nexial\nexial-core\src\test\resources\unittesting\artifact\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E476069-449A-481A-99A8-F364E3C1D79B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5846305-8B36-4553-95A5-625010CD53E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="623">
   <si>
     <t>target</t>
   </si>
@@ -1897,9 +1897,6 @@
     <t>Test UnitTesting</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>ProceedIf(${nexial.env} = UnitTesting)</t>
   </si>
   <si>
@@ -1919,6 +1916,21 @@
   </si>
   <si>
     <t>UnitTesting.Limit</t>
+  </si>
+  <si>
+    <t>assert var defined at project.properties loaded</t>
+  </si>
+  <si>
+    <t>assert var from project.properties is loaded has expected value</t>
+  </si>
+  <si>
+    <t>${Default.Name}</t>
+  </si>
+  <si>
+    <t>No1WorksHere</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
 </sst>
 </file>
@@ -2226,34 +2238,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
@@ -2289,6 +2273,34 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4752,12 +4764,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
@@ -4779,12 +4791,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.1" customHeight="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="36" t="s">
         <v>537</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="18" t="s">
         <v>538</v>
       </c>
@@ -4802,20 +4814,20 @@
       </c>
       <c r="J1" s="23"/>
       <c r="K1" s="14"/>
-      <c r="L1" s="29" t="s">
+      <c r="L1" s="38" t="s">
         <v>543</v>
       </c>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="30"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="39"/>
     </row>
     <row r="2" spans="1:15" ht="93" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="40" t="s">
         <v>544</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
@@ -4825,10 +4837,10 @@
       </c>
       <c r="J2" s="23"/>
       <c r="K2" s="14"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
     </row>
     <row r="3" spans="1:15" ht="9.9499999999999993" customHeight="1">
       <c r="A3" s="11"/>
@@ -4906,7 +4918,7 @@
         <v>350</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>611</v>
+        <v>622</v>
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -4923,13 +4935,13 @@
     </row>
     <row r="6" spans="1:15" ht="24" customHeight="1">
       <c r="A6" s="11"/>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="28" t="s">
         <v>609</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="30" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -4950,13 +4962,13 @@
     </row>
     <row r="7" spans="1:15" ht="24" customHeight="1">
       <c r="A7" s="11"/>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="31" t="s">
         <v>609</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="32" t="s">
         <v>40</v>
       </c>
       <c r="E7" s="17" t="s">
@@ -4977,13 +4989,13 @@
     </row>
     <row r="8" spans="1:15" ht="24" customHeight="1">
       <c r="A8" s="11"/>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="31" t="s">
         <v>608</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="32" t="s">
         <v>40</v>
       </c>
       <c r="E8" s="17" t="s">
@@ -5004,13 +5016,13 @@
     </row>
     <row r="9" spans="1:15" ht="24" customHeight="1">
       <c r="A9" s="11"/>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="31" t="s">
         <v>607</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="32" t="s">
         <v>269</v>
       </c>
       <c r="E9" s="17" t="s">
@@ -5029,14 +5041,14 @@
     </row>
     <row r="10" spans="1:15" ht="18.95" customHeight="1">
       <c r="A10" s="11"/>
-      <c r="B10" s="41" t="s">
-        <v>606</v>
-      </c>
-      <c r="C10" s="42" t="s">
+      <c r="B10" s="31" t="s">
+        <v>618</v>
+      </c>
+      <c r="C10" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="43" t="s">
-        <v>269</v>
+      <c r="D10" s="32" t="s">
+        <v>279</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>605</v>
@@ -5053,28 +5065,26 @@
       <c r="O10" s="14"/>
     </row>
     <row r="11" spans="1:15" ht="18.95" customHeight="1">
-      <c r="A11" s="11" t="s">
-        <v>610</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>615</v>
-      </c>
-      <c r="C11" s="16" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="33" t="s">
+        <v>619</v>
+      </c>
+      <c r="C11" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>350</v>
+      <c r="D11" s="35" t="s">
+        <v>40</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>611</v>
-      </c>
-      <c r="F11" s="17"/>
+        <v>621</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>620</v>
+      </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
-      <c r="J11" s="22" t="s">
-        <v>612</v>
-      </c>
+      <c r="J11" s="22"/>
       <c r="K11" s="14"/>
       <c r="L11" s="21"/>
       <c r="M11" s="13"/>
@@ -5082,26 +5092,28 @@
       <c r="O11" s="14"/>
     </row>
     <row r="12" spans="1:15" ht="18.95" customHeight="1">
-      <c r="A12" s="11"/>
-      <c r="B12" s="36" t="s">
-        <v>609</v>
-      </c>
-      <c r="C12" s="37" t="s">
+      <c r="A12" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>614</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="38" t="s">
-        <v>40</v>
+      <c r="D12" s="17" t="s">
+        <v>350</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>613</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>598</v>
-      </c>
+        <v>622</v>
+      </c>
+      <c r="F12" s="17"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
-      <c r="J12" s="22"/>
+      <c r="J12" s="22" t="s">
+        <v>611</v>
+      </c>
       <c r="K12" s="14"/>
       <c r="L12" s="21"/>
       <c r="M12" s="13"/>
@@ -5110,20 +5122,20 @@
     </row>
     <row r="13" spans="1:15" ht="18.95" customHeight="1">
       <c r="A13" s="11"/>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="28" t="s">
         <v>609</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="30" t="s">
         <v>40</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
@@ -5137,19 +5149,21 @@
     </row>
     <row r="14" spans="1:15" ht="18.95" customHeight="1">
       <c r="A14" s="11"/>
-      <c r="B14" s="39" t="s">
-        <v>608</v>
-      </c>
-      <c r="C14" s="35" t="s">
+      <c r="B14" s="31" t="s">
+        <v>609</v>
+      </c>
+      <c r="C14" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="40" t="s">
-        <v>269</v>
+      <c r="D14" s="32" t="s">
+        <v>40</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>618</v>
-      </c>
-      <c r="F14" s="17"/>
+        <v>613</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>601</v>
+      </c>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
@@ -5162,21 +5176,19 @@
     </row>
     <row r="15" spans="1:15" ht="18.95" customHeight="1">
       <c r="A15" s="11"/>
-      <c r="B15" s="39" t="s">
-        <v>607</v>
-      </c>
-      <c r="C15" s="35" t="s">
+      <c r="B15" s="31" t="s">
+        <v>608</v>
+      </c>
+      <c r="C15" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="D15" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>617</v>
       </c>
-      <c r="F15" s="17" t="s">
-        <v>616</v>
-      </c>
+      <c r="F15" s="17"/>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
@@ -5189,19 +5201,21 @@
     </row>
     <row r="16" spans="1:15" ht="18.95" customHeight="1">
       <c r="A16" s="11"/>
-      <c r="B16" s="41" t="s">
-        <v>606</v>
-      </c>
-      <c r="C16" s="42" t="s">
+      <c r="B16" s="31" t="s">
+        <v>607</v>
+      </c>
+      <c r="C16" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="43" t="s">
-        <v>269</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>605</v>
-      </c>
-      <c r="F16" s="17"/>
+      <c r="D16" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>615</v>
+      </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
@@ -5214,10 +5228,18 @@
     </row>
     <row r="17" spans="1:15" ht="18.95" customHeight="1">
       <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="B17" s="31" t="s">
+        <v>606</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>605</v>
+      </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
@@ -5231,11 +5253,21 @@
     </row>
     <row r="18" spans="1:15" ht="18.95" customHeight="1">
       <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
+      <c r="B18" s="33" t="s">
+        <v>619</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>621</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>620</v>
+      </c>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
@@ -5279,6 +5311,40 @@
       <c r="M20" s="13"/>
       <c r="N20" s="21"/>
       <c r="O20" s="14"/>
+    </row>
+    <row r="21" spans="1:15" ht="18.95" customHeight="1">
+      <c r="A21" s="11"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="14"/>
+    </row>
+    <row r="22" spans="1:15" ht="18.95" customHeight="1">
+      <c r="A22" s="11"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="14"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
@@ -5300,10 +5366,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C20" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C22" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D20" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D22" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>